<commit_message>
20221021 - Update jobfield.json                      -> fail_codes 추가
</commit_message>
<xml_diff>
--- a/ALLJOB.xlsx
+++ b/ALLJOB.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X97"/>
+  <dimension ref="A1:X98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +433,7 @@
     <col width="14.3" customWidth="1" min="10" max="10"/>
     <col width="18.7" customWidth="1" min="11" max="11"/>
     <col width="16.5" customWidth="1" min="12" max="12"/>
-    <col width="13.2" customWidth="1" min="13" max="13"/>
+    <col width="22" customWidth="1" min="13" max="13"/>
     <col width="18.7" customWidth="1" min="14" max="14"/>
     <col width="47.3" customWidth="1" min="15" max="15"/>
     <col width="50" customWidth="1" min="16" max="16"/>
@@ -6982,6 +6982,79 @@
         </is>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>APP_OBJECTS.Command_04</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>CMD</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>/app/Demo/batch_sleep.sh 10</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>db</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>root@db</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>su,mo,tu</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>10:00, 12:00, 14:00</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>APP_OBJECTS - Command_01</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr">
+        <is>
+          <t>/app/Demo/APP_OBJECTS/PRD/$AUTO_JOB_NAME.$AUTORUN.`date +%Y%m%d%H%M`.out</t>
+        </is>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>/app/Demo/APP_OBJECTS/PRD/$AUTO_JOB_NAME.$AUTORUN.`date +%Y%m%d%H%M`.err</t>
+        </is>
+      </c>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U98" t="inlineStr">
+        <is>
+          <t>APP_OBJECTS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>